<commit_message>
major reorganization and labeling
</commit_message>
<xml_diff>
--- a/inst/unit1_data/data_template.xlsx
+++ b/inst/unit1_data/data_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ehrli097\Desktop\AAA_2023\stats_book\inst\unit1_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4058490F-3A75-43C9-8EBA-9AF4C1C376E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F16B69B3-55AB-4E3B-B13A-5BC0BCF8C088}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{DA086CB5-4CC7-C543-B683-F95879B6D304}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="15">
   <si>
     <t>January</t>
   </si>
@@ -42,12 +42,6 @@
     <t>September</t>
   </si>
   <si>
-    <t>march</t>
-  </si>
-  <si>
-    <t>april</t>
-  </si>
-  <si>
     <t>Height_inches</t>
   </si>
   <si>
@@ -55,6 +49,36 @@
   </si>
   <si>
     <t>individual</t>
+  </si>
+  <si>
+    <t>March</t>
+  </si>
+  <si>
+    <t>April</t>
+  </si>
+  <si>
+    <t>October</t>
+  </si>
+  <si>
+    <t>November</t>
+  </si>
+  <si>
+    <t>June</t>
+  </si>
+  <si>
+    <t>December</t>
+  </si>
+  <si>
+    <t>February</t>
+  </si>
+  <si>
+    <t>July</t>
+  </si>
+  <si>
+    <t>August</t>
+  </si>
+  <si>
+    <t>May</t>
   </si>
 </sst>
 </file>
@@ -406,23 +430,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68E6F198-A363-294A-A85D-D79CC3A6139F}">
-  <dimension ref="A1:C53"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -452,7 +476,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C4">
         <v>72</v>
@@ -463,7 +487,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C5">
         <v>61</v>
@@ -473,240 +497,308 @@
       <c r="A6">
         <v>5</v>
       </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6">
+        <v>55</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7">
+        <v>65</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>72</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
+      <c r="B9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>75</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <v>69</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11">
+        <v>75</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
+      <c r="B12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>76</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13">
+        <v>70</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14">
+        <v>70</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15">
+        <v>69</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B23" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B25" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B27" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C28">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B29" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B30" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B31" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B32" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A34">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A35">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A36">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A37">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A38">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A39">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A40">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A41">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A42">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A43">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A44">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A45">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A46">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A47">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A48">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A49">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A50">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A51">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A52">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A53">
-        <v>52</v>
+      <c r="B33" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>